<commit_message>
added styling for graphs added age functions
</commit_message>
<xml_diff>
--- a/uploads/Authinticated_Example1.xlsx
+++ b/uploads/Authinticated_Example1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\MSPdata\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\mysitemsp\MSPdata\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="495">
   <si>
     <t>Customer ID</t>
   </si>
@@ -1446,6 +1446,69 @@
   </si>
   <si>
     <t>Mrs</t>
+  </si>
+  <si>
+    <t>20-05-1993</t>
+  </si>
+  <si>
+    <t>20-05-1994</t>
+  </si>
+  <si>
+    <t>20-05-1995</t>
+  </si>
+  <si>
+    <t>20-05-1996</t>
+  </si>
+  <si>
+    <t>20-05-1997</t>
+  </si>
+  <si>
+    <t>20-05-1998</t>
+  </si>
+  <si>
+    <t>20-05-1999</t>
+  </si>
+  <si>
+    <t>20-05-2000</t>
+  </si>
+  <si>
+    <t>20-05-2001</t>
+  </si>
+  <si>
+    <t>20-05-2002</t>
+  </si>
+  <si>
+    <t>20-05-1982</t>
+  </si>
+  <si>
+    <t>20-05-1983</t>
+  </si>
+  <si>
+    <t>20-05-1984</t>
+  </si>
+  <si>
+    <t>20-05-1985</t>
+  </si>
+  <si>
+    <t>20-05-1986</t>
+  </si>
+  <si>
+    <t>20-05-1987</t>
+  </si>
+  <si>
+    <t>20-05-1988</t>
+  </si>
+  <si>
+    <t>20-05-1989</t>
+  </si>
+  <si>
+    <t>20-05-1990</t>
+  </si>
+  <si>
+    <t>20-05-1991</t>
+  </si>
+  <si>
+    <t>20-05-1992</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1556,7 +1619,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1599,14 +1661,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>220</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:col>219</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>221</xdr:col>
-          <xdr:colOff>193399</xdr:colOff>
+          <xdr:col>220</xdr:col>
+          <xdr:colOff>101462</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -1646,14 +1708,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>220</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:col>219</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>221</xdr:col>
-          <xdr:colOff>193399</xdr:colOff>
+          <xdr:col>220</xdr:col>
+          <xdr:colOff>101462</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -1693,14 +1755,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>220</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:col>219</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>221</xdr:col>
-          <xdr:colOff>193399</xdr:colOff>
+          <xdr:col>220</xdr:col>
+          <xdr:colOff>101462</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -1740,14 +1802,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>220</xdr:col>
-          <xdr:colOff>511037</xdr:colOff>
+          <xdr:col>219</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>221</xdr:col>
-          <xdr:colOff>193399</xdr:colOff>
+          <xdr:col>220</xdr:col>
+          <xdr:colOff>101462</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -2052,8 +2114,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:KQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DK1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="DU11" sqref="DU11"/>
+    <sheetView tabSelected="1" topLeftCell="CP1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="DE11" sqref="DE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3022,8 +3084,8 @@
       <c r="DA2" t="s">
         <v>312</v>
       </c>
-      <c r="DE2" s="11">
-        <v>34005</v>
+      <c r="DE2" s="12" t="s">
+        <v>484</v>
       </c>
       <c r="DI2" t="s">
         <v>372</v>
@@ -3058,7 +3120,7 @@
       <c r="FA2" t="s">
         <v>395</v>
       </c>
-      <c r="FI2" s="12" t="s">
+      <c r="FI2" s="11" t="s">
         <v>419</v>
       </c>
       <c r="FM2" t="s">
@@ -3084,7 +3146,7 @@
       <c r="BE3" t="s">
         <v>312</v>
       </c>
-      <c r="BI3" s="13" t="s">
+      <c r="BI3" s="12" t="s">
         <v>315</v>
       </c>
       <c r="BM3" t="s">
@@ -3120,8 +3182,8 @@
       <c r="DA3" t="s">
         <v>311</v>
       </c>
-      <c r="DE3" s="11">
-        <v>34240</v>
+      <c r="DE3" s="12" t="s">
+        <v>485</v>
       </c>
       <c r="DI3" t="s">
         <v>373</v>
@@ -3156,10 +3218,10 @@
       <c r="FA3" t="s">
         <v>396</v>
       </c>
-      <c r="FI3" s="12" t="s">
+      <c r="FI3" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM3" s="13" t="s">
+      <c r="FM3" s="12" t="s">
         <v>420</v>
       </c>
       <c r="FQ3" t="s">
@@ -3168,10 +3230,10 @@
       <c r="FU3" t="s">
         <v>437</v>
       </c>
-      <c r="FY3" s="13" t="s">
+      <c r="FY3" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="HO3" s="13" t="s">
+      <c r="HO3" s="12" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3218,8 +3280,8 @@
       <c r="DA4" t="s">
         <v>312</v>
       </c>
-      <c r="DE4" s="11">
-        <v>34239</v>
+      <c r="DE4" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="DI4" t="s">
         <v>374</v>
@@ -3254,22 +3316,22 @@
       <c r="FA4" t="s">
         <v>397</v>
       </c>
-      <c r="FI4" s="12" t="s">
+      <c r="FI4" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM4" s="13" t="s">
+      <c r="FM4" s="12" t="s">
         <v>420</v>
       </c>
       <c r="FQ4" t="s">
         <v>423</v>
       </c>
-      <c r="FU4" s="13" t="s">
+      <c r="FU4" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="FY4" s="13" t="s">
+      <c r="FY4" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="HO4" s="13" t="s">
+      <c r="HO4" s="12" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3280,10 +3342,10 @@
       <c r="BE5" t="s">
         <v>311</v>
       </c>
-      <c r="BI5" s="13" t="s">
+      <c r="BI5" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ5" s="13" t="s">
+      <c r="BQ5" s="12" t="s">
         <v>322</v>
       </c>
       <c r="BU5" t="s">
@@ -3313,8 +3375,8 @@
       <c r="DA5" t="s">
         <v>311</v>
       </c>
-      <c r="DE5" s="11">
-        <v>34238</v>
+      <c r="DE5" s="12" t="s">
+        <v>487</v>
       </c>
       <c r="DI5" t="s">
         <v>375</v>
@@ -3349,22 +3411,22 @@
       <c r="FA5" t="s">
         <v>398</v>
       </c>
-      <c r="FI5" s="12" t="s">
+      <c r="FI5" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM5" s="13" t="s">
+      <c r="FM5" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="FQ5" s="13" t="s">
+      <c r="FQ5" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="FU5" s="13" t="s">
+      <c r="FU5" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="FY5" s="13" t="s">
+      <c r="FY5" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="HO5" s="13" t="s">
+      <c r="HO5" s="12" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3375,7 +3437,7 @@
       <c r="BE6" t="s">
         <v>314</v>
       </c>
-      <c r="BI6" s="13" t="s">
+      <c r="BI6" s="12" t="s">
         <v>316</v>
       </c>
       <c r="BQ6" t="s">
@@ -3408,8 +3470,8 @@
       <c r="DA6" t="s">
         <v>312</v>
       </c>
-      <c r="DE6" s="11">
-        <v>33872</v>
+      <c r="DE6" s="12" t="s">
+        <v>488</v>
       </c>
       <c r="DI6" t="s">
         <v>376</v>
@@ -3447,22 +3509,22 @@
       <c r="FA6" t="s">
         <v>399</v>
       </c>
-      <c r="FI6" s="12" t="s">
+      <c r="FI6" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM6" s="13" t="s">
+      <c r="FM6" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="FQ6" s="13" t="s">
+      <c r="FQ6" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="FU6" s="13" t="s">
+      <c r="FU6" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="FY6" s="13" t="s">
+      <c r="FY6" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="HO6" s="13" t="s">
+      <c r="HO6" s="12" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3473,7 +3535,7 @@
       <c r="BE7" t="s">
         <v>312</v>
       </c>
-      <c r="BI7" s="13" t="s">
+      <c r="BI7" s="12" t="s">
         <v>316</v>
       </c>
       <c r="BQ7" t="s">
@@ -3506,8 +3568,8 @@
       <c r="DA7" t="s">
         <v>311</v>
       </c>
-      <c r="DE7" s="11">
-        <v>34601</v>
+      <c r="DE7" s="12" t="s">
+        <v>489</v>
       </c>
       <c r="DI7" t="s">
         <v>378</v>
@@ -3545,22 +3607,22 @@
       <c r="FA7" t="s">
         <v>400</v>
       </c>
-      <c r="FI7" s="12" t="s">
+      <c r="FI7" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM7" s="13" t="s">
+      <c r="FM7" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="FQ7" s="13" t="s">
+      <c r="FQ7" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="FU7" s="13" t="s">
+      <c r="FU7" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="FY7" s="13" t="s">
+      <c r="FY7" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="HO7" s="13" t="s">
+      <c r="HO7" s="12" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3571,10 +3633,10 @@
       <c r="BE8" t="s">
         <v>311</v>
       </c>
-      <c r="BI8" s="13" t="s">
+      <c r="BI8" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="BQ8" s="13" t="s">
+      <c r="BQ8" s="12" t="s">
         <v>323</v>
       </c>
       <c r="BU8" t="s">
@@ -3602,13 +3664,13 @@
       <c r="DA8" t="s">
         <v>312</v>
       </c>
-      <c r="DE8" s="11">
-        <v>34235</v>
+      <c r="DE8" s="12" t="s">
+        <v>490</v>
       </c>
       <c r="DM8" t="s">
         <v>312</v>
       </c>
-      <c r="DQ8" s="13">
+      <c r="DQ8" s="12">
         <v>2021</v>
       </c>
       <c r="DU8" t="s">
@@ -3638,22 +3700,22 @@
       <c r="FA8" t="s">
         <v>401</v>
       </c>
-      <c r="FI8" s="12" t="s">
+      <c r="FI8" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM8" s="13" t="s">
+      <c r="FM8" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="FQ8" s="13" t="s">
+      <c r="FQ8" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="FU8" s="13" t="s">
+      <c r="FU8" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="FY8" s="13" t="s">
+      <c r="FY8" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="HO8" s="13" t="s">
+      <c r="HO8" s="12" t="s">
         <v>463</v>
       </c>
     </row>
@@ -3664,10 +3726,10 @@
       <c r="BE9" t="s">
         <v>313</v>
       </c>
-      <c r="BI9" s="13" t="s">
+      <c r="BI9" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="BQ9" s="13" t="s">
+      <c r="BQ9" s="12" t="s">
         <v>323</v>
       </c>
       <c r="BU9" t="s">
@@ -3697,8 +3759,8 @@
       <c r="DA9" t="s">
         <v>311</v>
       </c>
-      <c r="DE9" s="11">
-        <v>34234</v>
+      <c r="DE9" s="12" t="s">
+        <v>491</v>
       </c>
       <c r="DI9" t="s">
         <v>377</v>
@@ -3706,7 +3768,7 @@
       <c r="DM9" t="s">
         <v>371</v>
       </c>
-      <c r="DQ9" s="13">
+      <c r="DQ9" s="12">
         <v>2021</v>
       </c>
       <c r="DU9" t="s">
@@ -3736,36 +3798,39 @@
       <c r="FA9" t="s">
         <v>402</v>
       </c>
-      <c r="FI9" s="12" t="s">
+      <c r="FI9" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="FM9" s="13" t="s">
+      <c r="FM9" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="FQ9" s="13" t="s">
+      <c r="FQ9" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="FU9" s="13" t="s">
+      <c r="FU9" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="FY9" s="13" t="s">
+      <c r="FY9" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="HO9" s="13" t="s">
+      <c r="HO9" s="12" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="10" spans="1:303" x14ac:dyDescent="0.25">
-      <c r="BA10" s="13" t="s">
+      <c r="BA10" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="BI10" s="13" t="s">
+      <c r="BI10" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ10" s="13" t="s">
+      <c r="BQ10" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="DQ10" s="13">
+      <c r="DE10" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="DQ10" s="12">
         <v>2017</v>
       </c>
       <c r="DU10" t="s">
@@ -3774,42 +3839,45 @@
       <c r="EC10" t="s">
         <v>471</v>
       </c>
-      <c r="FQ10" s="13" t="s">
+      <c r="FQ10" s="12" t="s">
         <v>429</v>
       </c>
-      <c r="FU10" s="13" t="s">
+      <c r="FU10" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="FY10" s="13" t="s">
+      <c r="FY10" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="HO10" s="13" t="s">
+      <c r="HO10" s="12" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:303" x14ac:dyDescent="0.25">
-      <c r="BA11" s="13" t="s">
+      <c r="BA11" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="BI11" s="13" t="s">
+      <c r="BI11" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="BQ11" s="13" t="s">
+      <c r="BQ11" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="DQ11" s="13">
+      <c r="DE11" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="DQ11" s="12">
         <v>2017</v>
       </c>
-      <c r="EC11" s="13" t="s">
+      <c r="EC11" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="FQ11" s="13" t="s">
+      <c r="FQ11" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="FU11" s="13" t="s">
+      <c r="FU11" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="FY11" s="13" t="s">
+      <c r="FY11" s="12" t="s">
         <v>457</v>
       </c>
       <c r="HO11" t="s">
@@ -3817,28 +3885,31 @@
       </c>
     </row>
     <row r="12" spans="1:303" x14ac:dyDescent="0.25">
-      <c r="BA12" s="13" t="s">
+      <c r="BA12" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="BI12" s="13" t="s">
+      <c r="BI12" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ12" s="13" t="s">
+      <c r="BQ12" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="DQ12" s="13">
+      <c r="DE12" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="DQ12" s="12">
         <v>2017</v>
       </c>
-      <c r="EC12" s="13" t="s">
+      <c r="EC12" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="FQ12" s="13" t="s">
+      <c r="FQ12" s="12" t="s">
         <v>431</v>
       </c>
-      <c r="FU12" s="13" t="s">
+      <c r="FU12" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="FY12" s="13" t="s">
+      <c r="FY12" s="12" t="s">
         <v>458</v>
       </c>
       <c r="HO12" t="s">
@@ -3846,28 +3917,31 @@
       </c>
     </row>
     <row r="13" spans="1:303" x14ac:dyDescent="0.25">
-      <c r="BA13" s="13" t="s">
+      <c r="BA13" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="BI13" s="13" t="s">
+      <c r="BI13" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ13" s="13" t="s">
+      <c r="BQ13" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="DQ13" s="13">
+      <c r="DE13" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="DQ13" s="12">
         <v>2017</v>
       </c>
-      <c r="EC13" s="13" t="s">
+      <c r="EC13" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="FQ13" s="13" t="s">
+      <c r="FQ13" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="FU13" s="13" t="s">
+      <c r="FU13" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="FY13" s="13" t="s">
+      <c r="FY13" s="12" t="s">
         <v>459</v>
       </c>
       <c r="HO13" t="s">
@@ -3875,31 +3949,34 @@
       </c>
     </row>
     <row r="14" spans="1:303" x14ac:dyDescent="0.25">
-      <c r="BA14" s="13" t="s">
+      <c r="BA14" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="BI14" s="13" t="s">
+      <c r="BI14" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ14" s="13" t="s">
+      <c r="BQ14" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="DQ14" s="13">
+      <c r="DE14" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="DQ14" s="12">
         <v>2025</v>
       </c>
-      <c r="EC14" s="13" t="s">
+      <c r="EC14" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="FQ14" s="13" t="s">
+      <c r="FQ14" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="FU14" s="13" t="s">
+      <c r="FU14" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="FY14" s="13" t="s">
+      <c r="FY14" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="HO14" s="13" t="s">
+      <c r="HO14" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3907,54 +3984,60 @@
       <c r="BA15" t="s">
         <v>470</v>
       </c>
-      <c r="BI15" s="13" t="s">
+      <c r="BI15" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ15" s="13" t="s">
+      <c r="BQ15" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="DQ15" s="13">
+      <c r="DE15" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="DQ15" s="12">
         <v>2016</v>
       </c>
-      <c r="EC15" s="13" t="s">
+      <c r="EC15" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="FQ15" s="13" t="s">
+      <c r="FQ15" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="FU15" s="13" t="s">
+      <c r="FU15" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="FY15" s="13" t="s">
+      <c r="FY15" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="HO15" s="13" t="s">
+      <c r="HO15" s="12" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:303" x14ac:dyDescent="0.25">
-      <c r="BA16" s="13" t="s">
+      <c r="BA16" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="BI16" s="13" t="s">
+      <c r="BI16" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ16" s="13" t="s">
+      <c r="BQ16" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="DQ16" s="13">
+      <c r="DE16" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="DQ16" s="12">
         <v>2016</v>
       </c>
-      <c r="EC16" s="13" t="s">
+      <c r="EC16" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="FQ16" s="13" t="s">
+      <c r="FQ16" s="12" t="s">
         <v>435</v>
       </c>
-      <c r="FU16" s="13" t="s">
+      <c r="FU16" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="FY16" s="13" t="s">
+      <c r="FY16" s="12" t="s">
         <v>312</v>
       </c>
       <c r="HO16" t="s">
@@ -3962,19 +4045,22 @@
       </c>
     </row>
     <row r="17" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA17" s="13" t="s">
+      <c r="BA17" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="BI17" s="13" t="s">
+      <c r="BI17" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ17" s="13" t="s">
+      <c r="BQ17" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="DQ17" s="13">
+      <c r="DE17" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="DQ17" s="12">
         <v>2016</v>
       </c>
-      <c r="EC17" s="13" t="s">
+      <c r="EC17" s="12" t="s">
         <v>471</v>
       </c>
       <c r="HO17" t="s">
@@ -3982,197 +4068,215 @@
       </c>
     </row>
     <row r="18" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA18" s="13" t="s">
+      <c r="BA18" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="BI18" s="13" t="s">
+      <c r="BI18" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ18" s="13" t="s">
+      <c r="BQ18" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC18" s="13" t="s">
+      <c r="DE18" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="EC18" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="HO18" s="13" t="s">
+      <c r="HO18" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="HP18" s="13"/>
+      <c r="HP18" s="12"/>
     </row>
     <row r="19" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA19" s="13" t="s">
+      <c r="BA19" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="BI19" s="13" t="s">
+      <c r="BI19" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="BQ19" s="13" t="s">
+      <c r="BQ19" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC19" s="13" t="s">
+      <c r="DE19" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="EC19" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="HO19" s="13" t="s">
+      <c r="HO19" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="HP19" s="13"/>
+      <c r="HP19" s="12"/>
     </row>
     <row r="20" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA20" s="13" t="s">
+      <c r="BA20" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="BI20" s="13" t="s">
+      <c r="BI20" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="BQ20" s="13" t="s">
+      <c r="BQ20" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC20" s="13" t="s">
+      <c r="DE20" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="EC20" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="HO20" s="13" t="s">
+      <c r="HO20" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="HP20" s="13"/>
+      <c r="HP20" s="12"/>
     </row>
     <row r="21" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA21" s="13" t="s">
+      <c r="BA21" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="BI21" s="13" t="s">
+      <c r="BI21" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="BQ21" s="13" t="s">
+      <c r="BQ21" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC21" s="13" t="s">
+      <c r="DE21" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="EC21" s="12" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="22" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA22" s="13" t="s">
+      <c r="BA22" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="BI22" s="13" t="s">
+      <c r="BI22" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ22" s="13" t="s">
+      <c r="BQ22" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC22" s="13" t="s">
+      <c r="DE22" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="EC22" s="12" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="23" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA23" s="13" t="s">
+      <c r="BA23" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="BI23" s="13" t="s">
+      <c r="BI23" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ23" s="13" t="s">
+      <c r="BQ23" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC23" s="13" t="s">
+      <c r="DE23" s="12"/>
+      <c r="EC23" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="24" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA24" s="13" t="s">
+      <c r="BA24" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="BI24" s="13" t="s">
+      <c r="BI24" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ24" s="13" t="s">
+      <c r="BQ24" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="EC24" s="13" t="s">
+      <c r="DE24" s="12"/>
+      <c r="EC24" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="25" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA25" s="13" t="s">
+      <c r="BA25" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="BI25" s="13" t="s">
+      <c r="BI25" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ25" s="13" t="s">
+      <c r="BQ25" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC25" s="13" t="s">
+      <c r="DE25" s="12"/>
+      <c r="EC25" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="26" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA26" s="13" t="s">
+      <c r="BA26" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="BI26" s="13" t="s">
+      <c r="BI26" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="BQ26" s="13" t="s">
+      <c r="BQ26" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC26" s="13" t="s">
+      <c r="EC26" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="27" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA27" s="13" t="s">
+      <c r="BA27" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="BI27" s="13" t="s">
+      <c r="BI27" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ27" s="13" t="s">
+      <c r="BQ27" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="EC27" s="13" t="s">
+      <c r="EC27" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="28" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BA28" s="13" t="s">
+      <c r="BA28" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="BI28" s="13" t="s">
+      <c r="BI28" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="BQ28" s="13" t="s">
+      <c r="BQ28" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="EC28" s="13" t="s">
+      <c r="EC28" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="29" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BQ29" s="13" t="s">
+      <c r="BQ29" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="EC29" s="13" t="s">
+      <c r="EC29" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="30" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BQ30" s="13" t="s">
+      <c r="BQ30" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC30" s="13" t="s">
+      <c r="EC30" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="31" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BQ31" s="13" t="s">
+      <c r="BQ31" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="EC31" s="13" t="s">
+      <c r="EC31" s="12" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="32" spans="53:224" x14ac:dyDescent="0.25">
-      <c r="BQ32" s="13" t="s">
+      <c r="BQ32" s="12" t="s">
         <v>325</v>
       </c>
       <c r="EC32" t="s">
@@ -4180,132 +4284,132 @@
       </c>
     </row>
     <row r="33" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ33" s="13" t="s">
+      <c r="BQ33" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="34" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ34" s="13" t="s">
+      <c r="BQ34" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="35" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ35" s="13" t="s">
+      <c r="BQ35" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="36" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ36" s="13" t="s">
+      <c r="BQ36" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="37" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ37" s="13" t="s">
+      <c r="BQ37" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="38" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ38" s="13" t="s">
+      <c r="BQ38" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="39" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ39" s="13" t="s">
+      <c r="BQ39" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="40" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ40" s="13" t="s">
+      <c r="BQ40" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="41" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ41" s="13" t="s">
+      <c r="BQ41" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="42" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ42" s="13" t="s">
+      <c r="BQ42" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="43" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ43" s="13" t="s">
+      <c r="BQ43" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="44" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ44" s="13" t="s">
+      <c r="BQ44" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="45" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ45" s="13" t="s">
+      <c r="BQ45" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="46" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ46" s="13" t="s">
+      <c r="BQ46" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="47" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ47" s="13" t="s">
+      <c r="BQ47" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="48" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ48" s="13" t="s">
+      <c r="BQ48" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="49" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ49" s="13" t="s">
+      <c r="BQ49" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="50" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ50" s="13" t="s">
+      <c r="BQ50" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="51" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ51" s="13" t="s">
+      <c r="BQ51" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="52" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ52" s="13" t="s">
+      <c r="BQ52" s="12" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="53" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ53" s="13" t="s">
+      <c r="BQ53" s="12" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="54" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ54" s="13" t="s">
+      <c r="BQ54" s="12" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="55" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ55" s="13" t="s">
+      <c r="BQ55" s="12" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="56" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ56" s="13" t="s">
+      <c r="BQ56" s="12" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="57" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ57" s="13" t="s">
+      <c r="BQ57" s="12" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="58" spans="69:69" x14ac:dyDescent="0.25">
-      <c r="BQ58" s="13" t="s">
+      <c r="BQ58" s="12" t="s">
         <v>469</v>
       </c>
     </row>
@@ -4326,18 +4430,93 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId11" name="Control 1">
+        <control shapeId="1028" r:id="rId11" name="Control 4">
           <controlPr defaultSize="0" r:id="rId12">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>219</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>220</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId11" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId13" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>219</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>220</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId13" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId14" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>219</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>220</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId14" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId15" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>219</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>221</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
+                <xdr:col>220</xdr:col>
+                <xdr:colOff>104775</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </to>
@@ -4346,82 +4525,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId11" name="Control 1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId13" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>220</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>221</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId13" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId15" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>220</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>221</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId15" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId16" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>220</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>221</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId16" name="Control 4"/>
+        <control shapeId="1025" r:id="rId15" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
added Degree Added Download Table option
</commit_message>
<xml_diff>
--- a/uploads/Authinticated_Example1.xlsx
+++ b/uploads/Authinticated_Example1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="494">
   <si>
     <t>Customer ID</t>
   </si>
@@ -1500,6 +1500,12 @@
   </si>
   <si>
     <t>20-05-1992</t>
+  </si>
+  <si>
+    <t>aspire</t>
+  </si>
+  <si>
+    <t>Ph.D</t>
   </si>
 </sst>
 </file>
@@ -1652,14 +1658,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>218</xdr:col>
-          <xdr:colOff>327163</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>152814</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>219</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>448089</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -1699,14 +1705,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>218</xdr:col>
-          <xdr:colOff>327163</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>152814</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>219</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>448089</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -1746,14 +1752,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>218</xdr:col>
-          <xdr:colOff>327163</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>152814</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>219</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>448089</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -1793,14 +1799,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>218</xdr:col>
-          <xdr:colOff>327163</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>152814</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>187601</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>219</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:col>216</xdr:col>
+          <xdr:colOff>448089</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>111401</xdr:rowOff>
         </xdr:to>
@@ -2105,8 +2111,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:KQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CP1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="DF14" sqref="DF14"/>
+    <sheetView tabSelected="1" topLeftCell="EV1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="FI10" sqref="FI10:FI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,6 +3132,9 @@
       <c r="FY2" t="s">
         <v>451</v>
       </c>
+      <c r="GI2" t="s">
+        <v>492</v>
+      </c>
       <c r="HO2" t="s">
         <v>462</v>
       </c>
@@ -3224,6 +3233,9 @@
       <c r="FY3" s="12" t="s">
         <v>396</v>
       </c>
+      <c r="GI3" s="12" t="s">
+        <v>312</v>
+      </c>
       <c r="HO3" s="12" t="s">
         <v>462</v>
       </c>
@@ -3322,6 +3334,9 @@
       <c r="FY4" s="12" t="s">
         <v>452</v>
       </c>
+      <c r="GI4" s="12" t="s">
+        <v>312</v>
+      </c>
       <c r="HO4" s="12" t="s">
         <v>462</v>
       </c>
@@ -3417,6 +3432,9 @@
       <c r="FY5" s="12" t="s">
         <v>398</v>
       </c>
+      <c r="GI5" s="12" t="s">
+        <v>312</v>
+      </c>
       <c r="HO5" s="12" t="s">
         <v>462</v>
       </c>
@@ -3515,6 +3533,9 @@
       <c r="FY6" s="12" t="s">
         <v>453</v>
       </c>
+      <c r="GI6" s="12" t="s">
+        <v>492</v>
+      </c>
       <c r="HO6" s="12" t="s">
         <v>462</v>
       </c>
@@ -3613,6 +3634,9 @@
       <c r="FY7" s="12" t="s">
         <v>400</v>
       </c>
+      <c r="GI7" s="12" t="s">
+        <v>492</v>
+      </c>
       <c r="HO7" s="12" t="s">
         <v>462</v>
       </c>
@@ -3706,6 +3730,9 @@
       <c r="FY8" s="12" t="s">
         <v>454</v>
       </c>
+      <c r="GI8" s="12" t="s">
+        <v>492</v>
+      </c>
       <c r="HO8" s="12" t="s">
         <v>463</v>
       </c>
@@ -3804,6 +3831,9 @@
       <c r="FY9" s="12" t="s">
         <v>455</v>
       </c>
+      <c r="GI9" s="12" t="s">
+        <v>492</v>
+      </c>
       <c r="HO9" s="12" t="s">
         <v>463</v>
       </c>
@@ -3830,6 +3860,9 @@
       <c r="EC10" t="s">
         <v>471</v>
       </c>
+      <c r="FI10" s="11" t="s">
+        <v>493</v>
+      </c>
       <c r="FQ10" s="12" t="s">
         <v>429</v>
       </c>
@@ -3862,6 +3895,9 @@
       <c r="EC11" s="12" t="s">
         <v>471</v>
       </c>
+      <c r="FI11" s="11" t="s">
+        <v>493</v>
+      </c>
       <c r="FQ11" s="12" t="s">
         <v>430</v>
       </c>
@@ -3893,6 +3929,9 @@
       </c>
       <c r="EC12" s="12" t="s">
         <v>471</v>
+      </c>
+      <c r="FI12" s="11" t="s">
+        <v>493</v>
       </c>
       <c r="FQ12" s="12" t="s">
         <v>431</v>
@@ -4425,14 +4464,14 @@
           <controlPr defaultSize="0" r:id="rId12">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>218</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>219</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>447675</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </to>
@@ -4450,14 +4489,14 @@
           <controlPr defaultSize="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>218</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>12</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>219</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>447675</xdr:colOff>
                 <xdr:row>13</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </to>
@@ -4475,14 +4514,14 @@
           <controlPr defaultSize="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>218</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>15</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>219</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>447675</xdr:colOff>
                 <xdr:row>16</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </to>
@@ -4500,14 +4539,14 @@
           <controlPr defaultSize="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>218</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>15</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>219</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>216</xdr:col>
+                <xdr:colOff>447675</xdr:colOff>
                 <xdr:row>16</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </to>

</xml_diff>